<commit_message>
More functionality & comments to group Project
</commit_message>
<xml_diff>
--- a/projects/P1 -  Excel Grading/Well_Organized_Data_2.xlsx
+++ b/projects/P1 -  Excel Grading/Well_Organized_Data_2.xlsx
@@ -474,10 +474,6 @@
           <t>Highest Grade</t>
         </is>
       </c>
-      <c r="G2">
-        <f>MAX(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
-        <v/>
-      </c>
     </row>
     <row r="3">
       <c r="F3" t="inlineStr">
@@ -485,10 +481,6 @@
           <t>Lowest Grade</t>
         </is>
       </c>
-      <c r="G3">
-        <f>MIN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
-        <v/>
-      </c>
     </row>
     <row r="4">
       <c r="F4" t="inlineStr">
@@ -496,10 +488,6 @@
           <t>Mean Grade</t>
         </is>
       </c>
-      <c r="G4">
-        <f>IF(G6=0,0,AVERAGE(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
-        <v/>
-      </c>
     </row>
     <row r="5">
       <c r="F5" t="inlineStr">
@@ -507,20 +495,12 @@
           <t>Median Grade</t>
         </is>
       </c>
-      <c r="G5">
-        <f>IF(G6=0,0,MEDIAN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
-        <v/>
-      </c>
     </row>
     <row r="6">
       <c r="F6" t="inlineStr">
         <is>
           <t>Number of Students</t>
         </is>
-      </c>
-      <c r="G6">
-        <f>COUNT(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
-        <v/>
       </c>
     </row>
   </sheetData>
@@ -588,10 +568,6 @@
           <t>Highest Grade</t>
         </is>
       </c>
-      <c r="G2">
-        <f>MAX(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
-        <v/>
-      </c>
     </row>
     <row r="3">
       <c r="F3" t="inlineStr">
@@ -599,10 +575,6 @@
           <t>Lowest Grade</t>
         </is>
       </c>
-      <c r="G3">
-        <f>MIN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
-        <v/>
-      </c>
     </row>
     <row r="4">
       <c r="F4" t="inlineStr">
@@ -610,10 +582,6 @@
           <t>Mean Grade</t>
         </is>
       </c>
-      <c r="G4">
-        <f>IF(G6=0,0,AVERAGE(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
-        <v/>
-      </c>
     </row>
     <row r="5">
       <c r="F5" t="inlineStr">
@@ -621,20 +589,12 @@
           <t>Median Grade</t>
         </is>
       </c>
-      <c r="G5">
-        <f>IF(G6=0,0,MEDIAN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
-        <v/>
-      </c>
     </row>
     <row r="6">
       <c r="F6" t="inlineStr">
         <is>
           <t>Number of Students</t>
         </is>
-      </c>
-      <c r="G6">
-        <f>COUNT(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
-        <v/>
       </c>
     </row>
   </sheetData>
@@ -702,10 +662,6 @@
           <t>Highest Grade</t>
         </is>
       </c>
-      <c r="G2">
-        <f>MAX(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
-        <v/>
-      </c>
     </row>
     <row r="3">
       <c r="F3" t="inlineStr">
@@ -713,10 +669,6 @@
           <t>Lowest Grade</t>
         </is>
       </c>
-      <c r="G3">
-        <f>MIN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
-        <v/>
-      </c>
     </row>
     <row r="4">
       <c r="F4" t="inlineStr">
@@ -724,10 +676,6 @@
           <t>Mean Grade</t>
         </is>
       </c>
-      <c r="G4">
-        <f>IF(G6=0,0,AVERAGE(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
-        <v/>
-      </c>
     </row>
     <row r="5">
       <c r="F5" t="inlineStr">
@@ -735,20 +683,12 @@
           <t>Median Grade</t>
         </is>
       </c>
-      <c r="G5">
-        <f>IF(G6=0,0,MEDIAN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
-        <v/>
-      </c>
     </row>
     <row r="6">
       <c r="F6" t="inlineStr">
         <is>
           <t>Number of Students</t>
         </is>
-      </c>
-      <c r="G6">
-        <f>COUNT(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
-        <v/>
       </c>
     </row>
   </sheetData>
@@ -816,10 +756,6 @@
           <t>Highest Grade</t>
         </is>
       </c>
-      <c r="G2">
-        <f>MAX(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
-        <v/>
-      </c>
     </row>
     <row r="3">
       <c r="F3" t="inlineStr">
@@ -827,10 +763,6 @@
           <t>Lowest Grade</t>
         </is>
       </c>
-      <c r="G3">
-        <f>MIN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
-        <v/>
-      </c>
     </row>
     <row r="4">
       <c r="F4" t="inlineStr">
@@ -838,10 +770,6 @@
           <t>Mean Grade</t>
         </is>
       </c>
-      <c r="G4">
-        <f>IF(G6=0,0,AVERAGE(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
-        <v/>
-      </c>
     </row>
     <row r="5">
       <c r="F5" t="inlineStr">
@@ -849,20 +777,12 @@
           <t>Median Grade</t>
         </is>
       </c>
-      <c r="G5">
-        <f>IF(G6=0,0,MEDIAN(OFFSET($D$2,0,0,COUNT($D:$D)-1,1)))</f>
-        <v/>
-      </c>
     </row>
     <row r="6">
       <c r="F6" t="inlineStr">
         <is>
           <t>Number of Students</t>
         </is>
-      </c>
-      <c r="G6">
-        <f>COUNT(OFFSET($D$2,0,0,COUNT($D:$D)-1,1))</f>
-        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>